<commit_message>
implements contracts removes etm_key
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -7,10 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="gridconnections" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="gridnodes" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="actors" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="policies" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="CONVERSION" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="CONSUMPTION" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="PRODUCTION" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="STORAGE" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,220 +454,86 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>owner_actor</t>
+          <t>name</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>eta_r</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>capacity_kw</t>
+          <t>deliveryTemp_degc</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>parent_electric</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>parent_heat</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>assets</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>insulation_label</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>heating_type</t>
+          <t>capacityHeat_kW</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BUILDING</t>
+          <t>CONVERSION</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>LOGISTICS</t>
+          <t>GAS_BURNER</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BuildingGridConnection</t>
+          <t>ChemicalHeatConversionAsset</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>com1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>b1</t>
-        </is>
+          <t>Building_gas_burner_60kW</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.95</v>
       </c>
       <c r="F2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>E2</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>['Logistics_fleet_hgv_E', 'Building_solarpanels_0kWp', 'Building_gas_burner_60kW']</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>GASBURNER</t>
-        </is>
+        <v>90</v>
+      </c>
+      <c r="G2" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>INDUSTRY</t>
+          <t>CONVERSION</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>INDUSTRY_OTHER</t>
+          <t>GAS_BURNER</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>IndustryGridConnection</t>
+          <t>ChemicalHeatConversionAsset</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>com2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>b2</t>
-        </is>
+          <t>Building_gas_burner_60kW</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.95</v>
       </c>
       <c r="F3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>E2</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>['Building_solarpanels_0kWp', 'Building_gas_burner_60kW']</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>GASBURNER</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>SOLARFARM</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ProductionGridConnection</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>com3</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>b3</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>2000</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>E2</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>['Solarpanels_1MW', 'Solarpanels_1MW']</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>GRIDBATTERY</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ProductionGridConnection</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>com4</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>b4</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>E2</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>['Grid_battery_10MWh']</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+        <v>90</v>
+      </c>
+      <c r="G3" t="n">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -680,7 +546,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -706,90 +572,49 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>owner_actor</t>
+          <t>etm_key</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>capacity_kw</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>parent</t>
+          <t>yearlyDemandElectricity_kWh</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ELECTRICITY</t>
+          <t>CONSUMPTION</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MSLS</t>
+          <t>ELECTRICITY_DEMAND</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ElectricGridNode</t>
+          <t>ElectricConsumptionAsset</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>o1</t>
+          <t>logistics_fleet_e_hgv</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>E2</t>
+          <t>Logistics_fleet_hgv_E</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1200</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>E1</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ELECTRICITY</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>HSMS</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ElectricGridNode</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>o1</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>E1</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>500000</v>
-      </c>
-      <c r="G3" t="inlineStr"/>
+        <v>6500000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -802,7 +627,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -828,190 +653,138 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>etm_key</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>parent_actor</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>capacityElectricity_kW</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CONNECTIONOWNER</t>
+          <t>PRODUCTION</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>commercial</t>
+          <t>PHOTOVOLTAIC</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Actor</t>
+          <t>ElectricProductionAsset</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>com1</t>
+          <t>Solar panels for building, 0 kWp</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>hol1</t>
-        </is>
+          <t>Building_solarpanels_0kWp</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CONNECTIONOWNER</t>
+          <t>PRODUCTION</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>commercial</t>
+          <t>PHOTOVOLTAIC</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Actor</t>
+          <t>ElectricProductionAsset</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>com2</t>
+          <t>Solar panels for building, 0 kWp</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>hol1</t>
-        </is>
+          <t>Building_solarpanels_0kWp</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CONNECTIONOWNER</t>
+          <t>PRODUCTION</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>commercial</t>
+          <t>PHOTOVOLTAIC</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Actor</t>
+          <t>ElectricProductionAsset</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>com3</t>
+          <t>Solar field 1 MW</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>hol1</t>
-        </is>
+          <t>Solarpanels_1MW</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CONNECTIONOWNER</t>
+          <t>PRODUCTION</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>commercial</t>
+          <t>PHOTOVOLTAIC</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Actor</t>
+          <t>ElectricProductionAsset</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>com4</t>
+          <t>Solar field 1 MW</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>hol1</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ENERGYSUPPLIER</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Actor</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>sup1</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nat</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>ENERGYHOLON</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Actor</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>hol1</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>sup1</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>GRIDOPERATOR</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Actor</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>o1</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nat</t>
-        </is>
+          <t>Solarpanels_1MW</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -1025,7 +798,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1051,185 +824,54 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>parameter</t>
+          <t>name</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>capacityElectricity_kW</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>stateOfCharge_r</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>comment</t>
+          <t>storageCapacity_kWh</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>STORAGE_ELECTRIC</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Policy</t>
+          <t>ElectricStorageAsset</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>EV_charging_attitude_standard</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>CHEAP</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>charging behaviour not contingent on holon</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Policy</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Grid_MS_congestion_allowance_level_kW</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>kW</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>gridOperator policy variable</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Policy</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Grid_MS_congestion_price</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>kW</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>gridOperator policy value</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Policy</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Grid_MS_congestion_threshold</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0.7</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>fr</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>gridOperator policy value</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Policy</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Grid_MS_congestion_pricing_consumption</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>gridOperator policy value</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Policy</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Grid_MS_congestion_pricing_production</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>gridOperator policy value</t>
-        </is>
+          <t>Grid_battery_10MWh</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>